<commit_message>
Correção documentos e páginas do sistema
</commit_message>
<xml_diff>
--- a/Testes/Documento de Testes - MHS - 12.xlsx
+++ b/Testes/Documento de Testes - MHS - 12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Documentos\Meus Projetos\My Hair Salon\Testes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68329C45-CE85-4796-B9DC-84E9CE05F4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C73BDAE-F832-430F-BCC6-1B731B38540A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{60EB7970-8BE6-4BE5-9238-E82C81D98BC0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{60EB7970-8BE6-4BE5-9238-E82C81D98BC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Informações Gerais" sheetId="1" r:id="rId1"/>
@@ -90,9 +90,6 @@
     <t>Steps</t>
   </si>
   <si>
-    <t>Ambiente de desenvolvimento</t>
-  </si>
-  <si>
     <t>Gabriella Xavier</t>
   </si>
   <si>
@@ -170,6 +167,9 @@
   </si>
   <si>
     <t>O cursor do mouse deverá estar como pointer</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -254,9 +254,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -267,6 +264,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1007,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC0A0962-7C6C-4640-A9C3-D61D95AF0094}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1019,16 +1019,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4"/>
@@ -1038,7 +1038,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1046,7 +1046,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1054,7 +1054,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1062,14 +1062,14 @@
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="7">
         <v>45717</v>
       </c>
     </row>
@@ -1078,7 +1078,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1086,7 +1086,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -1110,7 +1110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E8ABBC-E64F-4728-8C3E-82E71C484C73}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -1118,40 +1118,40 @@
   <cols>
     <col min="1" max="1" width="11.88671875" style="5" customWidth="1"/>
     <col min="2" max="6" width="20.77734375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="20.77734375" style="11" customWidth="1"/>
+    <col min="7" max="7" width="20.77734375" style="10" customWidth="1"/>
     <col min="8" max="9" width="53.21875" style="5" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -1176,136 +1176,136 @@
         <v>10</v>
       </c>
       <c r="H6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>1</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="G7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
     </row>
     <row r="8" spans="1:9" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>2</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="10" t="s">
+      <c r="B8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
+      <c r="G8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
     </row>
     <row r="9" spans="1:9" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>3</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="10" t="s">
+      <c r="B9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+      <c r="G9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
     </row>
     <row r="10" spans="1:9" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>4</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="10" t="s">
+      <c r="B10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
+      <c r="F10" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
     </row>
     <row r="11" spans="1:9" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>5</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="B11" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
+      <c r="F11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
     </row>
   </sheetData>
   <autoFilter ref="A6:H6" xr:uid="{A5E8ABBC-E64F-4728-8C3E-82E71C484C73}"/>

</xml_diff>